<commit_message>
update them giao dien
</commit_message>
<xml_diff>
--- a/qt.xlsx
+++ b/qt.xlsx
@@ -18,13 +18,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -55,9 +58,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -423,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -432,199 +436,150 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Tên quy trình:</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>abc</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Bí danh:</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>abd</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Gắn vào TTHC:</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>12343</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>TTHC</t>
+        </is>
+      </c>
+      <c r="B5" s="1" t="inlineStr">
         <is>
           <t>Tên quy trình</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C5" s="1" t="inlineStr">
         <is>
           <t>Bí danh</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D5" s="1" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E5" s="1" t="inlineStr">
         <is>
           <t>Tên Form</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F5" s="1" t="inlineStr">
         <is>
           <t>Mã Action</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G5" s="1" t="inlineStr">
         <is>
           <t>Thời gian</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H5" s="1" t="inlineStr">
         <is>
           <t>Nhóm người dùng</t>
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr"/>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr">
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>12343</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>abc</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>abd</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Tiếp nhận hồ sơ</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>thêm mới</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Một cửa</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr">
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>them</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Thêm mới</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>12343</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>abc</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>abd</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Thẩm tra</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>chuyển xử lý</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Chuyên viên</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr"/>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Trình lãnh đạo</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>trình phê duyệt</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>lãnh đạo</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr"/>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Đóng dấu</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>chuyển ban hành</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>văn thư</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr"/>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Trả kết quả</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>chuyển trả kết quả</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>một cửa</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr"/>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Chuyển</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Chuyển xử lý</t>
+        </is>
+      </c>
       <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -637,7 +592,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -646,64 +601,20 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>Từ form</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>Đến form</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Tiếp nhận hồ sơ</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Thẩm tra</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Thẩm tra</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Trình lãnh đạo</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Trình lãnh đạo</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Đóng dấu</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Đóng dấu</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Trả kết quả</t>
-        </is>
-      </c>
+      <c r="A2" t="inlineStr"/>
+      <c r="B2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>